<commit_message>
Completed the testing tables
</commit_message>
<xml_diff>
--- a/docs/Lab2/TakeHome/Lab02_BBT_Form.xlsx
+++ b/docs/Lab2/TakeHome/Lab02_BBT_Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrei\SSVV\MavenApp\docs\Lab2\TakeHome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B715294B-B043-46DA-993B-43024F261F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967072B8-D6C4-4EC9-A83E-FF7D631294B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="935" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem" sheetId="5" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t xml:space="preserve">Statement: </t>
   </si>
@@ -343,14 +343,38 @@
     <t>11, 13</t>
   </si>
   <si>
-    <t xml:space="preserve">   n</t>
+    <t>group &gt;= 0</t>
+  </si>
+  <si>
+    <t>MAXINT - 1</t>
+  </si>
+  <si>
+    <t>MAXINT</t>
+  </si>
+  <si>
+    <t>MAXINT + 1</t>
+  </si>
+  <si>
+    <t>MAXINT-1</t>
+  </si>
+  <si>
+    <t>MAXINT+1</t>
+  </si>
+  <si>
+    <t>Student added</t>
+  </si>
+  <si>
+    <t>Student created</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,15 +443,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
@@ -445,23 +460,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -846,9 +844,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -861,8 +859,7 @@
       <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
@@ -874,10 +871,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,17 +881,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,20 +937,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -936,52 +964,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1393,7 +1403,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B5" sqref="B5:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1405,170 +1415,170 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="48">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="48"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="48">
+      <c r="B4" s="22">
         <v>2</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="48">
+      <c r="B5" s="22">
         <v>3</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="48">
+      <c r="B6" s="22">
         <v>4</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="48">
+      <c r="B7" s="22">
         <v>5</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="48">
+      <c r="B8" s="22">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="48">
+      <c r="B9" s="22">
         <v>7</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="48">
+      <c r="B10" s="22">
         <v>8</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="48">
+      <c r="B11" s="22">
         <v>9</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="48"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="48">
+      <c r="B12" s="22">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="48">
+      <c r="B13" s="22">
         <v>11</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="48"/>
+      <c r="E13" s="22"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="48">
+      <c r="B14" s="22">
         <v>12</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="48">
+      <c r="B15" s="22">
         <v>13</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="48"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="48">
+      <c r="B16" s="22">
         <v>14</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1588,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:J18"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,26 +1611,26 @@
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11"/>
-      <c r="C2" s="27" t="s">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="10"/>
+      <c r="C2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="29"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="G2" s="35"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
@@ -1630,237 +1640,232 @@
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="50">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="23">
         <v>1</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="24">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="52"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="50">
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="23">
         <v>2</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="24">
         <v>2</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="24">
         <v>-12</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="50">
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="23">
         <v>3</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="52"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="50">
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="23">
         <v>4</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="24">
         <v>4</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="52"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="50">
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
         <v>5</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="24">
         <v>6</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="52"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="50">
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
         <v>6</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="52"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="50">
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="23">
         <v>7</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="24">
         <v>8</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="52"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="50">
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="23">
         <v>8</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="24">
         <v>10</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="52"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="50">
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="23">
         <v>9</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="52"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="50">
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="23">
         <v>10</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="24">
         <v>12</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="52"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="54">
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="27">
         <v>11</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="28">
         <v>14</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="56"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="29"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1882,7 +1887,7 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1905,99 +1910,113 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="31">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-1</v>
+      </c>
     </row>
     <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="32"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="33"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="31">
+      <c r="B9" s="37">
         <v>2</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="32"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="32"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="32"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="32"/>
-      <c r="C13" s="30"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="33"/>
-      <c r="C14" s="30"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="31">
+      <c r="B15" s="37">
         <v>3</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="32"/>
-      <c r="C16" s="30"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="32"/>
-      <c r="C17" s="30"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="32"/>
-      <c r="C18" s="30"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="32"/>
-      <c r="C19" s="30"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="33"/>
-      <c r="C20" s="30"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="5"/>
     </row>
   </sheetData>
@@ -2018,12 +2037,13 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F24"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
     <col min="6" max="6" width="32.109375" customWidth="1"/>
     <col min="8" max="8" width="68.33203125" customWidth="1"/>
   </cols>
@@ -2031,188 +2051,242 @@
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="5">
+        <v>7</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="B5" s="49">
+        <v>1</v>
+      </c>
+      <c r="C5" s="50">
+        <v>1</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="51">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="15"/>
+      <c r="B6" s="49">
+        <v>2</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="51">
+        <v>0</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="49">
+        <v>3</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="51">
+        <v>1</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="5"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="B8" s="49">
+        <v>4</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
+      <c r="B9" s="49">
+        <v>5</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="51"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="5"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="49">
+        <v>6</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="5"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="5"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="5"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="5"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="5"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
     </row>
     <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="5"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="5"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="16"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="5"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="5"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="5"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="16"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="5"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2232,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,14 +2327,14 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="36"/>
+      <c r="G2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="30"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
@@ -2272,104 +2346,333 @@
       <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="58">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="58">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="58">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="58">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>11</v>
+      </c>
+      <c r="C14" s="58">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>12</v>
+      </c>
+      <c r="C15" s="58">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="58">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>14</v>
+      </c>
+      <c r="C17" s="58">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>15</v>
+      </c>
+      <c r="C18" s="58">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2385,7 +2688,7 @@
   <dimension ref="B2:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,81 +2698,81 @@
   <sheetData>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="19" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="42"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="46" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="46"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <f>SUM(D6:E6)</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="21" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="1">
@@ -2477,10 +2780,15 @@
         <v>0</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="22"/>
+      <c r="K6" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="G4:G5"/>
@@ -2488,11 +2796,6 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented the first 8/9 test cases. Fixed bug in validator regarding check order.
</commit_message>
<xml_diff>
--- a/docs/Lab2/TakeHome/Lab02_BBT_Form.xlsx
+++ b/docs/Lab2/TakeHome/Lab02_BBT_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrei\SSVV\MavenApp\docs\Lab2\TakeHome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967072B8-D6C4-4EC9-A83E-FF7D631294B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5474366-A9F2-46DC-9C80-AAE165CCEACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="935" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t xml:space="preserve">Statement: </t>
   </si>
@@ -235,12 +235,6 @@
     <t>Req_a)</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>not yet</t>
-  </si>
-  <si>
     <t>Add a student</t>
   </si>
   <si>
@@ -368,19 +362,44 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Can't be implemented because MAXINT+1 result in negative number</t>
+  </si>
+  <si>
+    <t>NullPointerException</t>
+  </si>
+  <si>
+    <t>ValidationException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student added </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -451,21 +470,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -488,6 +492,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -497,7 +534,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -841,25 +878,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
@@ -871,9 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -881,36 +925,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -937,13 +990,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -952,46 +1032,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1350,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1363,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1371,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1382,7 +1438,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1390,7 +1446,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1415,171 +1471,171 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="20">
+        <v>2</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="20">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="20">
+        <v>4</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="22" t="s">
+    </row>
+    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="20">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="22">
-        <v>2</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22" t="s">
+      <c r="D7" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="20">
+        <v>6</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="22">
-        <v>3</v>
-      </c>
-      <c r="C5" s="30" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="20">
+        <v>7</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="22">
-        <v>4</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="22">
-        <v>5</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="20">
+        <v>8</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="20">
+        <v>9</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="22">
-        <v>6</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="22">
-        <v>7</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="D11" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="20">
+        <v>10</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="20">
+        <v>11</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="22">
-        <v>8</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="22">
-        <v>9</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="D13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="20">
+        <v>12</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="20">
+        <v>13</v>
+      </c>
+      <c r="C15" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="22">
-        <v>10</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="22">
-        <v>11</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="22">
-        <v>12</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="22">
-        <v>13</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="22"/>
+      <c r="D15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="22">
+      <c r="B16" s="20">
         <v>14</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22" t="s">
-        <v>54</v>
+      <c r="C16" s="31"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1601,7 +1657,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,28 +1670,28 @@
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="35"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -1646,223 +1702,223 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="23">
+      <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="22">
         <v>1</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="22">
+        <v>12</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="21">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="22">
+        <v>-12</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="21">
+        <v>3</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="21">
+        <v>4</v>
+      </c>
+      <c r="C7" s="22">
+        <v>4</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="21">
+        <v>5</v>
+      </c>
+      <c r="C8" s="22">
+        <v>6</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="21">
+        <v>6</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="21">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22">
+        <v>8</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
+        <v>8</v>
+      </c>
+      <c r="C11" s="22">
+        <v>10</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="21">
+        <v>9</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="21">
+        <v>10</v>
+      </c>
+      <c r="C13" s="22">
         <v>12</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="23">
-        <v>2</v>
-      </c>
-      <c r="C5" s="24">
-        <v>2</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="24">
-        <v>-12</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
-        <v>3</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="23">
-        <v>4</v>
-      </c>
-      <c r="C7" s="24">
-        <v>4</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="24" t="s">
+      <c r="D13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="25">
+        <v>11</v>
+      </c>
+      <c r="C14" s="26">
+        <v>14</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="23">
-        <v>5</v>
-      </c>
-      <c r="C8" s="24">
-        <v>6</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="23">
-        <v>6</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="23">
-        <v>7</v>
-      </c>
-      <c r="C10" s="24">
-        <v>8</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="23">
-        <v>8</v>
-      </c>
-      <c r="C11" s="24">
-        <v>10</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="23">
-        <v>9</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="23">
-        <v>10</v>
-      </c>
-      <c r="C13" s="24">
-        <v>12</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="27">
-        <v>11</v>
-      </c>
-      <c r="C14" s="28">
-        <v>14</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="29"/>
+      <c r="F14" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="27"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="8" t="s">
@@ -1910,113 +1966,113 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="37">
+      <c r="B3" s="38">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>74</v>
+      <c r="C3" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="D3" s="5">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="38"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="38"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="39"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="40"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="38"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="39"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="37">
+      <c r="B9" s="38">
         <v>2</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="38"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="38"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="38"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="38"/>
-      <c r="C13" s="36"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="39"/>
-      <c r="C14" s="36"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="37">
+      <c r="B15" s="38">
         <v>3</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="38"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="38"/>
-      <c r="C17" s="36"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="38"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="38"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="39"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="5"/>
     </row>
   </sheetData>
@@ -2034,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2051,28 +2107,28 @@
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5">
         <v>7</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>14</v>
@@ -2083,221 +2139,235 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="49">
+      <c r="B5" s="28">
         <v>1</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="41">
         <v>1</v>
       </c>
-      <c r="D5" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="51">
+      <c r="D5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="29">
         <v>-1</v>
       </c>
-      <c r="F5" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="51"/>
+      <c r="F5" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="49">
+      <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="51">
+      <c r="C6" s="41"/>
+      <c r="D6" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="29">
         <v>0</v>
       </c>
-      <c r="F6" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="51"/>
+      <c r="F6" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="49">
+      <c r="B7" s="28">
         <v>3</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="51">
+      <c r="C7" s="41"/>
+      <c r="D7" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="29">
         <v>1</v>
       </c>
-      <c r="F7" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="51"/>
+      <c r="F7" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="49">
+      <c r="B8" s="28">
         <v>4</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="51"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="49">
+      <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="51"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="49">
+      <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="51"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="49"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="49"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="49"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="49"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="49"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="49"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="49"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-    </row>
-    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="49"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-    </row>
-    <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="49"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-    </row>
-    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="49"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="49"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-    </row>
-    <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="49"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="49"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="28"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="28"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="28"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="28"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="28"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="28"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="C17:C22"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2306,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,25 +2388,27 @@
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" customWidth="1"/>
+    <col min="9" max="9" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2347,10 +2419,10 @@
         <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>14</v>
@@ -2359,325 +2431,375 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4">
+    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="56">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="56">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="56">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="56">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="56">
+        <v>2</v>
+      </c>
+      <c r="C5" s="56">
+        <v>1</v>
+      </c>
+      <c r="D5" s="56">
+        <v>2</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="56">
+        <v>0</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="56">
+        <v>3</v>
+      </c>
+      <c r="C6" s="56">
+        <v>1</v>
+      </c>
+      <c r="D6" s="56">
+        <v>3</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="57">
+        <v>1</v>
+      </c>
+      <c r="G6" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="56">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>1</v>
+      </c>
+      <c r="D7" s="56">
+        <v>4</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="56">
+        <v>5</v>
+      </c>
+      <c r="C8" s="56">
+        <v>1</v>
+      </c>
+      <c r="D8" s="56">
+        <v>5</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="58">
+        <v>6</v>
+      </c>
+      <c r="C9" s="58">
+        <v>2</v>
+      </c>
+      <c r="D9" s="58">
+        <v>6</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="56"/>
+      <c r="I9" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="56">
+        <v>7</v>
+      </c>
+      <c r="C10" s="59">
+        <v>3</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F10" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="56">
+        <v>8</v>
+      </c>
+      <c r="C11" s="59">
+        <v>4</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F11" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="56">
+        <v>9</v>
+      </c>
+      <c r="C12" s="59">
+        <v>5</v>
+      </c>
+      <c r="D12" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="E12" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="F12" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="56">
+        <v>10</v>
+      </c>
+      <c r="C13" s="59">
+        <v>6</v>
+      </c>
+      <c r="D13" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="14" t="s">
+      <c r="E13" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H13" s="56"/>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="56">
+        <v>11</v>
+      </c>
+      <c r="C14" s="59">
+        <v>7</v>
+      </c>
+      <c r="D14" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="E14" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="56"/>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="56">
+        <v>12</v>
+      </c>
+      <c r="C15" s="59">
+        <v>8</v>
+      </c>
+      <c r="D15" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="58">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="E15" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="56"/>
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="56">
+        <v>13</v>
+      </c>
+      <c r="C16" s="59">
+        <v>9</v>
+      </c>
+      <c r="D16" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="58">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="58" t="s">
+      <c r="E16" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="56"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="56">
+        <v>14</v>
+      </c>
+      <c r="C17" s="59">
+        <v>10</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="56"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="56">
+        <v>15</v>
+      </c>
+      <c r="C18" s="59">
+        <v>11</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12" s="58">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="4">
-        <v>10</v>
-      </c>
-      <c r="C13" s="58">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="4">
-        <v>11</v>
-      </c>
-      <c r="C14" s="58">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="4">
-        <v>12</v>
-      </c>
-      <c r="C15" s="58">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="4">
-        <v>13</v>
-      </c>
-      <c r="C16" s="58">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="4">
-        <v>14</v>
-      </c>
-      <c r="C17" s="58">
-        <v>10</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
-        <v>15</v>
-      </c>
-      <c r="C18" s="58">
-        <v>11</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="5"/>
+      <c r="G18" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="56"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2688,7 +2810,7 @@
   <dimension ref="B2:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2698,97 +2820,102 @@
   <sheetData>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="16" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="42"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="49" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <f>SUM(D6:E6)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="I6" s="1">
         <f>SUM(J6:K6)</f>
+        <v>8</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="17">
         <v>0</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="G4:G5"/>
@@ -2796,6 +2923,11 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>